<commit_message>
Entropy & Inner Product Experiments
</commit_message>
<xml_diff>
--- a/Experiments/Previous Experiments/2019 07 09/Accumalation.xlsx
+++ b/Experiments/Previous Experiments/2019 07 09/Accumalation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuval\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yuval\Desktop\Distributed Monitoring Thesis\Experiments\Previous Experiments\2019 07 09\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009969D8-ED61-4E43-B47F-A1431EEF3068}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79BEE20A-7D71-4DA5-B68A-93AE0BFF4442}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1038,6 +1038,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:trendlineType val="linear"/>
+            <c:intercept val="0"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="0"/>
           </c:trendline>
@@ -1730,6 +1731,8 @@
         <c:axId val="447042287"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="80000"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1933,10 +1936,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:schemeClr val="tx1"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -3029,19 +3029,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>8.4102664837000587E-2</c:v>
+                  <c:v>0.92242186320089359</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0001353884311053E-2</c:v>
+                  <c:v>0.97087251024363141</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9.7322299007533628E-2</c:v>
+                  <c:v>0.9113092852523309</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.0639022731645179E-2</c:v>
+                  <c:v>0.96094801190044843</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.2863816182711095E-2</c:v>
+                  <c:v>0.9588979735248564</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3134,19 +3134,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3239,19 +3239,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.40825439978200101</c:v>
+                  <c:v>0.7100989708640717</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.44402084302056216</c:v>
+                  <c:v>0.69251077976702069</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.65212514121340548</c:v>
+                  <c:v>0.60528102566464703</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.46467908444817835</c:v>
+                  <c:v>0.68274341500326163</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46859218206072839</c:v>
+                  <c:v>0.68092422948677289</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3344,19 +3344,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.57664867736424408</c:v>
+                  <c:v>0.63425670814105894</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0318583375118995</c:v>
+                  <c:v>0.49216029559646579</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3668907197166165</c:v>
+                  <c:v>0.42249521351781216</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.3426378165009747</c:v>
+                  <c:v>0.42686922961639295</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.368078864126882</c:v>
+                  <c:v>0.42228323353103492</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3449,19 +3449,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0.12863914373204824</c:v>
+                  <c:v>0.88602278731297612</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.13097885250604568</c:v>
+                  <c:v>0.88418983059159761</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.2453289806883269</c:v>
+                  <c:v>0.80300066529189174</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.14658851666727349</c:v>
+                  <c:v>0.87215246399523139</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14954229392357496</c:v>
+                  <c:v>0.869911446743588</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3511,7 +3511,7 @@
           </c:marker>
           <c:trendline>
             <c:spPr>
-              <a:ln w="19050" cap="rnd">
+              <a:ln w="28575" cap="rnd">
                 <a:solidFill>
                   <a:schemeClr val="accent6"/>
                 </a:solidFill>
@@ -3554,19 +3554,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6241,16 +6241,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6803,7 +6803,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{897AF533-400B-425A-B826-168F88C388CF}" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{897AF533-400B-425A-B826-168F88C388CF}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:I10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -8716,8 +8716,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E4EE27C-097E-4F42-A3BF-D0A5817E1153}">
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A1:G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9363,8 +9363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3526F6D8-7520-4F93-ADB7-A882DB114AA7}">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9815,28 +9815,28 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <f t="shared" ref="B23:F23" si="0">(B9-MIN(B16,B9))/(B16-B2)</f>
-        <v>8.4102664837000587E-2</v>
+        <f>(MIN(B16,B9)-B2)/(B9-B2)</f>
+        <v>0.92242186320089359</v>
       </c>
       <c r="C23">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f t="shared" ref="C23:G23" si="0">(MIN(C16,C9)-C2)/(C9-C2)</f>
+        <v>1</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>0.40825439978200101</v>
+        <v>0.7100989708640717</v>
       </c>
       <c r="E23">
         <f t="shared" si="0"/>
-        <v>0.57664867736424408</v>
+        <v>0.63425670814105894</v>
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>0.12863914373204824</v>
+        <v>0.88602278731297612</v>
       </c>
       <c r="G23">
-        <f>(G9-MIN(G16,G9))/(G16-G2)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -9844,28 +9844,28 @@
         <v>100</v>
       </c>
       <c r="B24">
-        <f t="shared" ref="B24:G24" si="1">(B10-MIN(B17,B10))/(B17-B3)</f>
-        <v>3.0001353884311053E-2</v>
+        <f t="shared" ref="B24:G24" si="1">(MIN(B17,B10)-B3)/(B10-B3)</f>
+        <v>0.97087251024363141</v>
       </c>
       <c r="C24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24">
         <f t="shared" si="1"/>
-        <v>0.44402084302056216</v>
+        <v>0.69251077976702069</v>
       </c>
       <c r="E24">
         <f t="shared" si="1"/>
-        <v>1.0318583375118995</v>
+        <v>0.49216029559646579</v>
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>0.13097885250604568</v>
+        <v>0.88418983059159761</v>
       </c>
       <c r="G24">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -9873,28 +9873,28 @@
         <v>225</v>
       </c>
       <c r="B25">
-        <f t="shared" ref="B25:G25" si="2">(B11-MIN(B18,B11))/(B18-B4)</f>
-        <v>9.7322299007533628E-2</v>
+        <f t="shared" ref="B25:G25" si="2">(MIN(B18,B11)-B4)/(B11-B4)</f>
+        <v>0.9113092852523309</v>
       </c>
       <c r="C25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25">
         <f t="shared" si="2"/>
-        <v>0.65212514121340548</v>
+        <v>0.60528102566464703</v>
       </c>
       <c r="E25">
         <f t="shared" si="2"/>
-        <v>1.3668907197166165</v>
+        <v>0.42249521351781216</v>
       </c>
       <c r="F25">
         <f t="shared" si="2"/>
-        <v>0.2453289806883269</v>
+        <v>0.80300066529189174</v>
       </c>
       <c r="G25">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -9902,28 +9902,28 @@
         <v>400</v>
       </c>
       <c r="B26">
-        <f t="shared" ref="B26:G26" si="3">(B12-MIN(B19,B12))/(B19-B5)</f>
-        <v>4.0639022731645179E-2</v>
+        <f t="shared" ref="B26:G26" si="3">(MIN(B19,B12)-B5)/(B12-B5)</f>
+        <v>0.96094801190044843</v>
       </c>
       <c r="C26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D26">
         <f t="shared" si="3"/>
-        <v>0.46467908444817835</v>
+        <v>0.68274341500326163</v>
       </c>
       <c r="E26">
         <f t="shared" si="3"/>
-        <v>1.3426378165009747</v>
+        <v>0.42686922961639295</v>
       </c>
       <c r="F26">
         <f t="shared" si="3"/>
-        <v>0.14658851666727349</v>
+        <v>0.87215246399523139</v>
       </c>
       <c r="G26">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -9931,28 +9931,28 @@
         <v>625</v>
       </c>
       <c r="B27">
-        <f t="shared" ref="B27:G27" si="4">(B13-MIN(B20,B13))/(B20-B6)</f>
-        <v>4.2863816182711095E-2</v>
+        <f t="shared" ref="B27:G27" si="4">(MIN(B20,B13)-B6)/(B13-B6)</f>
+        <v>0.9588979735248564</v>
       </c>
       <c r="C27">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27">
         <f t="shared" si="4"/>
-        <v>0.46859218206072839</v>
+        <v>0.68092422948677289</v>
       </c>
       <c r="E27">
         <f t="shared" si="4"/>
-        <v>1.368078864126882</v>
+        <v>0.42228323353103492</v>
       </c>
       <c r="F27">
         <f t="shared" si="4"/>
-        <v>0.14954229392357496</v>
+        <v>0.869911446743588</v>
       </c>
       <c r="G27">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>